<commit_message>
added theory upper and lower limit lambda bottle
</commit_message>
<xml_diff>
--- a/PW/lambda_bottle.xlsx
+++ b/PW/lambda_bottle.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUTD Term 3\2D\green-fingers-2d\PW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WKieee\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12547" windowHeight="6213" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>T_i</t>
   </si>
@@ -74,6 +74,63 @@
   <si>
     <t>Specific Heat Capacity of Water/J g^-1 K^-1</t>
   </si>
+  <si>
+    <t>R_convwater</t>
+  </si>
+  <si>
+    <t>lambda_water</t>
+  </si>
+  <si>
+    <t>R_condglass</t>
+  </si>
+  <si>
+    <t>lambda_glass</t>
+  </si>
+  <si>
+    <t>R_air</t>
+  </si>
+  <si>
+    <t>lambda_air</t>
+  </si>
+  <si>
+    <t>1/hA</t>
+  </si>
+  <si>
+    <t>L/kA</t>
+  </si>
+  <si>
+    <t>lower limit</t>
+  </si>
+  <si>
+    <t>upper limit</t>
+  </si>
+  <si>
+    <t>lower limit h_water</t>
+  </si>
+  <si>
+    <t>upper limit h_water</t>
+  </si>
+  <si>
+    <t>lower limit h_air</t>
+  </si>
+  <si>
+    <t>upper limit h_air</t>
+  </si>
+  <si>
+    <t>http://www.hcheattransfer.com/coefficients.html</t>
+  </si>
+  <si>
+    <t>lower limit k_plexi</t>
+  </si>
+  <si>
+    <t>upper limit k_plexi</t>
+  </si>
+  <si>
+    <t>https://www.electronics-cooling.com/2001/05/the-thermal-conductivity-of-unfilled-plastics/</t>
+  </si>
+  <si>
+    <t>lambda bottle theory</t>
+  </si>
 </sst>
 </file>
 
@@ -84,13 +141,25 @@
     <numFmt numFmtId="165" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,13 +182,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3111,19 +3182,19 @@
   <dimension ref="A1:K191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.9375" style="2"/>
-    <col min="3" max="3" width="8.9375" style="1"/>
-    <col min="5" max="5" width="8.9375" style="1"/>
-    <col min="7" max="7" width="15.64453125" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3143,7 +3214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42.7</v>
       </c>
@@ -3169,7 +3240,7 @@
         <v>26.270666666666653</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42.6</v>
       </c>
@@ -3191,7 +3262,7 @@
         <v>16.329333333333349</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42.4</v>
       </c>
@@ -3213,7 +3284,7 @@
         <v>16.129333333333346</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42.2</v>
       </c>
@@ -3235,7 +3306,7 @@
         <v>15.92933333333335</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>42</v>
       </c>
@@ -3257,7 +3328,7 @@
         <v>15.729333333333347</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>41.9</v>
       </c>
@@ -3279,7 +3350,7 @@
         <v>15.629333333333346</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>41.8</v>
       </c>
@@ -3301,7 +3372,7 @@
         <v>15.529333333333344</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>41.7</v>
       </c>
@@ -3323,7 +3394,7 @@
         <v>15.42933333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>41.6</v>
       </c>
@@ -3345,7 +3416,7 @@
         <v>15.329333333333349</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>41.5</v>
       </c>
@@ -3367,7 +3438,7 @@
         <v>15.229333333333347</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>41.4</v>
       </c>
@@ -3389,7 +3460,7 @@
         <v>15.129333333333346</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>41.3</v>
       </c>
@@ -3411,7 +3482,7 @@
         <v>15.029333333333344</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>41.2</v>
       </c>
@@ -3433,7 +3504,7 @@
         <v>14.92933333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>41.1</v>
       </c>
@@ -3455,7 +3526,7 @@
         <v>14.829333333333349</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>41</v>
       </c>
@@ -3477,7 +3548,7 @@
         <v>14.729333333333347</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>40.9</v>
       </c>
@@ -3499,7 +3570,7 @@
         <v>14.629333333333346</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>40.799999999999997</v>
       </c>
@@ -3521,7 +3592,7 @@
         <v>14.529333333333344</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>40.700000000000003</v>
       </c>
@@ -3543,7 +3614,7 @@
         <v>14.42933333333335</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>40.6</v>
       </c>
@@ -3565,7 +3636,7 @@
         <v>14.329333333333349</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>40.5</v>
       </c>
@@ -3587,7 +3658,7 @@
         <v>14.229333333333347</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>40.4</v>
       </c>
@@ -3609,7 +3680,7 @@
         <v>14.129333333333346</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>40.299999999999997</v>
       </c>
@@ -3631,7 +3702,7 @@
         <v>14.029333333333344</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>40.200000000000003</v>
       </c>
@@ -3653,7 +3724,7 @@
         <v>13.92933333333335</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>40.1</v>
       </c>
@@ -3675,7 +3746,7 @@
         <v>13.829333333333349</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>40</v>
       </c>
@@ -3697,7 +3768,7 @@
         <v>13.729333333333347</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>39.9</v>
       </c>
@@ -3719,7 +3790,7 @@
         <v>13.629333333333346</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>39.799999999999997</v>
       </c>
@@ -3741,7 +3812,7 @@
         <v>13.529333333333344</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>39.700000000000003</v>
       </c>
@@ -3763,7 +3834,7 @@
         <v>13.42933333333335</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>39.6</v>
       </c>
@@ -3785,7 +3856,7 @@
         <v>13.329333333333349</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>39.5</v>
       </c>
@@ -3807,7 +3878,7 @@
         <v>13.229333333333347</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>39.4</v>
       </c>
@@ -3829,7 +3900,7 @@
         <v>13.129333333333346</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>39.299999999999997</v>
       </c>
@@ -3851,7 +3922,7 @@
         <v>13.029333333333344</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>39.200000000000003</v>
       </c>
@@ -3873,7 +3944,7 @@
         <v>12.92933333333335</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>39.1</v>
       </c>
@@ -3895,7 +3966,7 @@
         <v>12.829333333333349</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>39</v>
       </c>
@@ -3917,7 +3988,7 @@
         <v>12.729333333333347</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>38.9</v>
       </c>
@@ -3939,7 +4010,7 @@
         <v>12.629333333333346</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>38.799999999999997</v>
       </c>
@@ -3961,7 +4032,7 @@
         <v>12.529333333333344</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38.700000000000003</v>
       </c>
@@ -3983,7 +4054,7 @@
         <v>12.42933333333335</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38.6</v>
       </c>
@@ -4005,7 +4076,7 @@
         <v>12.329333333333349</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38.5</v>
       </c>
@@ -4027,7 +4098,7 @@
         <v>12.229333333333347</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>38.4</v>
       </c>
@@ -4049,7 +4120,7 @@
         <v>12.129333333333346</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>38.299999999999997</v>
       </c>
@@ -4071,7 +4142,7 @@
         <v>12.029333333333344</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>38.200000000000003</v>
       </c>
@@ -4093,7 +4164,7 @@
         <v>11.92933333333335</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>38.1</v>
       </c>
@@ -4115,7 +4186,7 @@
         <v>11.829333333333349</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>38</v>
       </c>
@@ -4137,7 +4208,7 @@
         <v>11.729333333333347</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>37.9</v>
       </c>
@@ -4159,7 +4230,7 @@
         <v>11.629333333333346</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>37.799999999999997</v>
       </c>
@@ -4181,7 +4252,7 @@
         <v>11.529333333333344</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>37.700000000000003</v>
       </c>
@@ -4206,7 +4277,7 @@
         <v>5.2822530159999997E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>37.6</v>
       </c>
@@ -4228,7 +4299,7 @@
         <v>11.329333333333349</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>37.5</v>
       </c>
@@ -4250,7 +4321,7 @@
         <v>11.229333333333347</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>37.4</v>
       </c>
@@ -4272,7 +4343,7 @@
         <v>11.129333333333346</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>37.299999999999997</v>
       </c>
@@ -4294,7 +4365,7 @@
         <v>11.029333333333344</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>37.200000000000003</v>
       </c>
@@ -4316,7 +4387,7 @@
         <v>10.92933333333335</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>37.1</v>
       </c>
@@ -4338,7 +4409,7 @@
         <v>10.829333333333349</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>37</v>
       </c>
@@ -4360,7 +4431,7 @@
         <v>10.729333333333347</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>36.9</v>
       </c>
@@ -4382,7 +4453,7 @@
         <v>10.629333333333346</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>36.799999999999997</v>
       </c>
@@ -4404,7 +4475,7 @@
         <v>10.529333333333344</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>36.700000000000003</v>
       </c>
@@ -4426,7 +4497,7 @@
         <v>10.42933333333335</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>36.6</v>
       </c>
@@ -4448,7 +4519,7 @@
         <v>10.329333333333349</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>36.5</v>
       </c>
@@ -4470,7 +4541,7 @@
         <v>10.229333333333347</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>36.4</v>
       </c>
@@ -4492,7 +4563,7 @@
         <v>10.129333333333346</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>36.299999999999997</v>
       </c>
@@ -4514,7 +4585,7 @@
         <v>10.029333333333344</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>36.200000000000003</v>
       </c>
@@ -4536,7 +4607,7 @@
         <v>9.92933333333335</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>36.1</v>
       </c>
@@ -4558,7 +4629,7 @@
         <v>9.8293333333333486</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>36</v>
       </c>
@@ -4580,7 +4651,7 @@
         <v>9.7293333333333472</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>35.9</v>
       </c>
@@ -4602,7 +4673,7 @@
         <v>9.6293333333333457</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>35.799999999999997</v>
       </c>
@@ -4624,7 +4695,7 @@
         <v>9.5293333333333443</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>35.700000000000003</v>
       </c>
@@ -4646,7 +4717,7 @@
         <v>9.42933333333335</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>35.6</v>
       </c>
@@ -4668,7 +4739,7 @@
         <v>9.3293333333333486</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>35.5</v>
       </c>
@@ -4690,7 +4761,7 @@
         <v>9.2293333333333472</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>35.4</v>
       </c>
@@ -4712,7 +4783,7 @@
         <v>9.1293333333333457</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>35.299999999999997</v>
       </c>
@@ -4734,7 +4805,7 @@
         <v>9.0293333333333443</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>35.200000000000003</v>
       </c>
@@ -4756,7 +4827,7 @@
         <v>8.92933333333335</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>35.1</v>
       </c>
@@ -4778,7 +4849,7 @@
         <v>8.8293333333333486</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>35</v>
       </c>
@@ -4800,577 +4871,577 @@
         <v>8.7293333333333472</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D77">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D78">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D79">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D80">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D81">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D82">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D83">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D84">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D85">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D86">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D87">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D88">
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D89">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D90">
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D91">
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D92">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D93">
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D94">
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D95">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D96">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D97">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D98">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D99">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D100">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D101">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D102">
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D103">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D104">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D105">
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D106">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D107">
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D108">
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D109">
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D110">
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D111">
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D112">
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113">
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114">
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115">
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D116">
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D117">
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D118">
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D119">
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D120">
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121">
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122">
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123">
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D124">
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D125">
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D126">
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D127">
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128">
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129">
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130">
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131">
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132">
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133">
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134">
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135">
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136">
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137">
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138">
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139">
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140">
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141">
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142">
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143">
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144">
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145">
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146">
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148">
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149">
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151">
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D152">
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D153">
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D154">
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D155">
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D156">
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D157">
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D158">
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D159">
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D160">
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D161">
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D162">
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D163">
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D164">
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D165">
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D166">
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D167">
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D168">
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D169">
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D170">
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171">
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D172">
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D173">
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D174">
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D175">
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D176">
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D177">
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D178">
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D179">
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D180">
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D181">
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D182">
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D183">
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D184">
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D185">
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D186">
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D187">
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D188">
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D189">
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D190">
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D191">
         <v>2</v>
       </c>
@@ -5383,27 +5454,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.05859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.52734375" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="3">
         <v>5.2822530159999997E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <f>1/($G$15*$B$14*10^-4)</f>
+        <v>0.27837473693587356</v>
+      </c>
+      <c r="I2">
+        <f>1/(G16*B14*10^-4)</f>
+        <v>9.2791578978624514E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5411,8 +5507,35 @@
         <f>(B1*B10*B8*B9)^-1</f>
         <v>1.514216957373038</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <f>1/$H$2</f>
+        <v>3.5922800000000006</v>
+      </c>
+      <c r="I3">
+        <f>1/I2</f>
+        <v>10.776840000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <f>B6*10^-3/(G19*B14*10^-4)</f>
+        <v>0.57312445839738679</v>
+      </c>
+      <c r="I4">
+        <f>(B6*10^-3)/(G20*B14*10^-4)</f>
+        <v>0.51279556803976711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5425,16 +5548,54 @@
       <c r="D5">
         <v>46.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <f>1/H4</f>
+        <v>1.7448217142857143</v>
+      </c>
+      <c r="I5">
+        <f>1/I4</f>
+        <v>1.9500948571428574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+        <v>1.4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <f>1/(I15*B14*10^-4)</f>
+        <v>6.9593684233968389</v>
+      </c>
+      <c r="I6">
+        <f>1/(I16*B14*10^-4)</f>
+        <v>3.4796842116984195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <f>1/H6</f>
+        <v>0.14369120000000002</v>
+      </c>
+      <c r="I7">
+        <f>1/I6</f>
+        <v>0.28738240000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -5442,15 +5603,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <v>0.997</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9">
+        <f>1/(H2+H4+H6)</f>
+        <v>0.12802675052410903</v>
+      </c>
+      <c r="I9">
+        <f>1/(I2+I4+I6)</f>
+        <v>0.24478178123132099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -5458,16 +5630,16 @@
         <v>4.18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <f>B6*0.001/(B3*2*(B5*C5+B5*D5+C5*D5)*0.000001)</f>
-        <v>0.1961965344013846</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+        <f>B6*0.001/(B3*(2*(B5*C5+C5*D5)+B5*D5)*0.000001)</f>
+        <v>0.2077835445403923</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5475,7 +5647,21 @@
         <v>143.69120000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>250</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5483,8 +5669,48 @@
         <f>B14*(1/B3)/(2*0.01*(B5*C5+B5*D5+C5*D5))</f>
         <v>1.7619822164985144</v>
       </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16">
+        <v>750</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="7"/>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
in range with the practical lambda algaebottle
</commit_message>
<xml_diff>
--- a/PW/lambda_bottle.xlsx
+++ b/PW/lambda_bottle.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUTD Term 3\2D\green-fingers-2d\PW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WKieee\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9087" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>T_i</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Specific Heat Capacity of Water/J g^-1 K^-1</t>
-  </si>
-  <si>
-    <t>R_convwater</t>
   </si>
   <si>
     <t>lambda_water</t>
@@ -132,31 +129,28 @@
     <t>lambda bottle theory</t>
   </si>
   <si>
-    <t>at 50 deg C</t>
+    <t>lower limit h_water25</t>
   </si>
   <si>
-    <t>Thermal Conductance/W K^-1</t>
+    <t>upper limit h_water25</t>
   </si>
   <si>
-    <t>bottle</t>
+    <t>R_convwater_25</t>
   </si>
   <si>
-    <t>tubing</t>
+    <t>R_convwater_35</t>
   </si>
   <si>
-    <t>exponential coeff</t>
+    <t>http://www.engineeringtoolbox.com/convective-heat-transfer-d_430.html</t>
   </si>
   <si>
-    <t>CALCULATOR</t>
+    <t>forced convection</t>
   </si>
   <si>
-    <t>volume of water (ml)</t>
+    <t>free convection</t>
   </si>
   <si>
-    <t>Experimental results</t>
-  </si>
-  <si>
-    <t>lambda</t>
+    <t>never used</t>
   </si>
 </sst>
 </file>
@@ -168,7 +162,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,23 +183,9 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,12 +200,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -233,223 +213,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1080,21 +863,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="el-GR" sz="3200" b="0" i="1" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Δ</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-SG" sz="3200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>T/K against Time/s</a:t>
+              <a:rPr lang="en-SG"/>
+              <a:t>delta T/K against Time/s</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1103,8 +873,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.30619109392625854"/>
-          <c:y val="3.3452283169723013E-2"/>
+          <c:x val="0.3324293122755364"/>
+          <c:y val="3.3067969866776292E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1153,8 +923,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="3"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -1171,11 +941,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000">
-                    <a:alpha val="55000"/>
-                  </a:srgbClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="solid"/>
+                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1185,67 +953,10 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.4131925712742523E-2"/>
-                  <c:y val="-0.32993255938674509"/>
+                  <c:x val="-8.9969312939782373E-2"/>
+                  <c:y val="0.12406909028838597"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="2800" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>y = 1.5829607582E+01e</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="2800" baseline="30000">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>-5.2822530160E-03x</a:t>
-                    </a:r>
-                    <a:br>
-                      <a:rPr lang="en-US" sz="2800" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                      </a:rPr>
-                    </a:br>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="2800" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>R² = 9.9648425472E-01</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="2800">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="0.0000000000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1766,7 +1477,6 @@
         <c:axId val="710102688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="120"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1799,32 +1509,6 @@
           </c:spPr>
         </c:minorGridlines>
         <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-SG" sz="2000">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>Time/s</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1838,9 +1522,12 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1851,7 +1538,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1873,9 +1560,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1927,55 +1617,6 @@
           </c:spPr>
         </c:minorGridlines>
         <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="el-GR" sz="2000" b="0" i="1" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Δ</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-SG" sz="2000" b="0" i="1" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>T</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-SG" sz="2000" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>/K</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-SG" sz="2000">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1989,9 +1630,12 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2002,7 +1646,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2024,9 +1668,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2039,8 +1686,6 @@
         <c:crossAx val="710102688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
-        <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3240,15 +2885,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>95253</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>61384</xdr:rowOff>
+      <xdr:colOff>332316</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>402166</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>105834</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>330201</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>55034</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3576,19 +3221,19 @@
   <dimension ref="A1:K191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q29" sqref="Q29"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.87890625" style="2"/>
-    <col min="3" max="3" width="8.87890625" style="1"/>
-    <col min="5" max="5" width="8.87890625" style="1"/>
-    <col min="7" max="7" width="15.64453125" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42.7</v>
       </c>
@@ -3629,12 +3274,12 @@
         <f>A2-$G$2</f>
         <v>16.42933333333335</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <f>AVERAGE(B:B)</f>
         <v>26.270666666666653</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42.6</v>
       </c>
@@ -3656,7 +3301,7 @@
         <v>16.329333333333349</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42.4</v>
       </c>
@@ -3678,7 +3323,7 @@
         <v>16.129333333333346</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42.2</v>
       </c>
@@ -3700,7 +3345,7 @@
         <v>15.92933333333335</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>42</v>
       </c>
@@ -3722,7 +3367,7 @@
         <v>15.729333333333347</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>41.9</v>
       </c>
@@ -3744,7 +3389,7 @@
         <v>15.629333333333346</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>41.8</v>
       </c>
@@ -3766,7 +3411,7 @@
         <v>15.529333333333344</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>41.7</v>
       </c>
@@ -3788,7 +3433,7 @@
         <v>15.42933333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>41.6</v>
       </c>
@@ -3810,7 +3455,7 @@
         <v>15.329333333333349</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>41.5</v>
       </c>
@@ -3832,7 +3477,7 @@
         <v>15.229333333333347</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>41.4</v>
       </c>
@@ -3854,7 +3499,7 @@
         <v>15.129333333333346</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>41.3</v>
       </c>
@@ -3876,7 +3521,7 @@
         <v>15.029333333333344</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>41.2</v>
       </c>
@@ -3898,7 +3543,7 @@
         <v>14.92933333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>41.1</v>
       </c>
@@ -3920,7 +3565,7 @@
         <v>14.829333333333349</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>41</v>
       </c>
@@ -3942,7 +3587,7 @@
         <v>14.729333333333347</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>40.9</v>
       </c>
@@ -3964,7 +3609,7 @@
         <v>14.629333333333346</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>40.799999999999997</v>
       </c>
@@ -3986,7 +3631,7 @@
         <v>14.529333333333344</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>40.700000000000003</v>
       </c>
@@ -4008,7 +3653,7 @@
         <v>14.42933333333335</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>40.6</v>
       </c>
@@ -4030,7 +3675,7 @@
         <v>14.329333333333349</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>40.5</v>
       </c>
@@ -4052,7 +3697,7 @@
         <v>14.229333333333347</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>40.4</v>
       </c>
@@ -4074,7 +3719,7 @@
         <v>14.129333333333346</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>40.299999999999997</v>
       </c>
@@ -4096,7 +3741,7 @@
         <v>14.029333333333344</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>40.200000000000003</v>
       </c>
@@ -4118,7 +3763,7 @@
         <v>13.92933333333335</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>40.1</v>
       </c>
@@ -4140,7 +3785,7 @@
         <v>13.829333333333349</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>40</v>
       </c>
@@ -4162,7 +3807,7 @@
         <v>13.729333333333347</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>39.9</v>
       </c>
@@ -4184,7 +3829,7 @@
         <v>13.629333333333346</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>39.799999999999997</v>
       </c>
@@ -4206,7 +3851,7 @@
         <v>13.529333333333344</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>39.700000000000003</v>
       </c>
@@ -4228,7 +3873,7 @@
         <v>13.42933333333335</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>39.6</v>
       </c>
@@ -4250,7 +3895,7 @@
         <v>13.329333333333349</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>39.5</v>
       </c>
@@ -4272,7 +3917,7 @@
         <v>13.229333333333347</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>39.4</v>
       </c>
@@ -4294,7 +3939,7 @@
         <v>13.129333333333346</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>39.299999999999997</v>
       </c>
@@ -4316,7 +3961,7 @@
         <v>13.029333333333344</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>39.200000000000003</v>
       </c>
@@ -4338,7 +3983,7 @@
         <v>12.92933333333335</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>39.1</v>
       </c>
@@ -4360,7 +4005,7 @@
         <v>12.829333333333349</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>39</v>
       </c>
@@ -4382,7 +4027,7 @@
         <v>12.729333333333347</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>38.9</v>
       </c>
@@ -4404,7 +4049,7 @@
         <v>12.629333333333346</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>38.799999999999997</v>
       </c>
@@ -4426,7 +4071,7 @@
         <v>12.529333333333344</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38.700000000000003</v>
       </c>
@@ -4448,7 +4093,7 @@
         <v>12.42933333333335</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38.6</v>
       </c>
@@ -4470,7 +4115,7 @@
         <v>12.329333333333349</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38.5</v>
       </c>
@@ -4492,7 +4137,7 @@
         <v>12.229333333333347</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>38.4</v>
       </c>
@@ -4514,7 +4159,7 @@
         <v>12.129333333333346</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>38.299999999999997</v>
       </c>
@@ -4536,7 +4181,7 @@
         <v>12.029333333333344</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>38.200000000000003</v>
       </c>
@@ -4558,7 +4203,7 @@
         <v>11.92933333333335</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>38.1</v>
       </c>
@@ -4580,7 +4225,7 @@
         <v>11.829333333333349</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>38</v>
       </c>
@@ -4602,7 +4247,7 @@
         <v>11.729333333333347</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>37.9</v>
       </c>
@@ -4624,7 +4269,7 @@
         <v>11.629333333333346</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>37.799999999999997</v>
       </c>
@@ -4646,7 +4291,7 @@
         <v>11.529333333333344</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>37.700000000000003</v>
       </c>
@@ -4671,7 +4316,7 @@
         <v>5.2822530159999997E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>37.6</v>
       </c>
@@ -4693,7 +4338,7 @@
         <v>11.329333333333349</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>37.5</v>
       </c>
@@ -4715,7 +4360,7 @@
         <v>11.229333333333347</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>37.4</v>
       </c>
@@ -4737,7 +4382,7 @@
         <v>11.129333333333346</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>37.299999999999997</v>
       </c>
@@ -4759,7 +4404,7 @@
         <v>11.029333333333344</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>37.200000000000003</v>
       </c>
@@ -4781,7 +4426,7 @@
         <v>10.92933333333335</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>37.1</v>
       </c>
@@ -4803,7 +4448,7 @@
         <v>10.829333333333349</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>37</v>
       </c>
@@ -4825,7 +4470,7 @@
         <v>10.729333333333347</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>36.9</v>
       </c>
@@ -4847,7 +4492,7 @@
         <v>10.629333333333346</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>36.799999999999997</v>
       </c>
@@ -4869,7 +4514,7 @@
         <v>10.529333333333344</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>36.700000000000003</v>
       </c>
@@ -4891,7 +4536,7 @@
         <v>10.42933333333335</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>36.6</v>
       </c>
@@ -4913,7 +4558,7 @@
         <v>10.329333333333349</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>36.5</v>
       </c>
@@ -4935,7 +4580,7 @@
         <v>10.229333333333347</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>36.4</v>
       </c>
@@ -4957,7 +4602,7 @@
         <v>10.129333333333346</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>36.299999999999997</v>
       </c>
@@ -4979,7 +4624,7 @@
         <v>10.029333333333344</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>36.200000000000003</v>
       </c>
@@ -5001,7 +4646,7 @@
         <v>9.92933333333335</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>36.1</v>
       </c>
@@ -5023,7 +4668,7 @@
         <v>9.8293333333333486</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>36</v>
       </c>
@@ -5045,7 +4690,7 @@
         <v>9.7293333333333472</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>35.9</v>
       </c>
@@ -5067,7 +4712,7 @@
         <v>9.6293333333333457</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>35.799999999999997</v>
       </c>
@@ -5089,7 +4734,7 @@
         <v>9.5293333333333443</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>35.700000000000003</v>
       </c>
@@ -5111,7 +4756,7 @@
         <v>9.42933333333335</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>35.6</v>
       </c>
@@ -5133,7 +4778,7 @@
         <v>9.3293333333333486</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>35.5</v>
       </c>
@@ -5155,7 +4800,7 @@
         <v>9.2293333333333472</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>35.4</v>
       </c>
@@ -5177,7 +4822,7 @@
         <v>9.1293333333333457</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>35.299999999999997</v>
       </c>
@@ -5199,7 +4844,7 @@
         <v>9.0293333333333443</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>35.200000000000003</v>
       </c>
@@ -5221,7 +4866,7 @@
         <v>8.92933333333335</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>35.1</v>
       </c>
@@ -5243,7 +4888,7 @@
         <v>8.8293333333333486</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>35</v>
       </c>
@@ -5265,577 +4910,577 @@
         <v>8.7293333333333472</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D77">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D78">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D79">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D80">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D81">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D82">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D83">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D84">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D85">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D86">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D87">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D88">
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D89">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D90">
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D91">
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D92">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D93">
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D94">
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D95">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D96">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D97">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D98">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D99">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D100">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D101">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D102">
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D103">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D104">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D105">
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D106">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D107">
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D108">
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D109">
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D110">
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D111">
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D112">
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113">
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114">
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115">
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D116">
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D117">
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D118">
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D119">
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D120">
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121">
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122">
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123">
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D124">
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D125">
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D126">
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D127">
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128">
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129">
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130">
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131">
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132">
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133">
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134">
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135">
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136">
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137">
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138">
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139">
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140">
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141">
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142">
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143">
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144">
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145">
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146">
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148">
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149">
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151">
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D152">
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D153">
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D154">
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D155">
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D156">
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D157">
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D158">
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D159">
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D160">
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D161">
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D162">
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D163">
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D164">
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D165">
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D166">
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D167">
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D168">
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D169">
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D170">
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171">
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D172">
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D173">
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D174">
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D175">
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D176">
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D177">
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D178">
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D179">
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D180">
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D181">
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D182">
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D183">
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D184">
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D185">
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D186">
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D187">
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D188">
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D189">
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D190">
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.5">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D191">
         <v>2</v>
       </c>
@@ -5848,393 +5493,321 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.3515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.52734375" customWidth="1"/>
-    <col min="7" max="7" width="18.234375" customWidth="1"/>
-    <col min="9" max="9" width="13.76171875" customWidth="1"/>
-    <col min="10" max="10" width="12.64453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="31" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="B1" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="B1" s="3">
         <v>5.2822530159999997E-3</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="I2" t="s">
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B3" s="11"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="12"/>
-      <c r="G3" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2">
+        <f>1/($G$16*$B$14*10^-4)</f>
+        <v>1.3918736846793678</v>
+      </c>
+      <c r="I2">
+        <f>1/(G17*B14*10^-4)</f>
+        <v>6.9593684233968398E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>(B1*B10*B8*B9)^-1</f>
+        <v>1.514216957373038</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <f>1/$H$2</f>
+        <v>0.71845600000000009</v>
+      </c>
+      <c r="I3">
+        <f>1/I2</f>
+        <v>143.69120000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="I3">
-        <f>1/($H$17*$C$16*10^-4)</f>
-        <v>0.27837473693587356</v>
-      </c>
-      <c r="J3">
-        <f>1/(H18*C16*10^-4)</f>
-        <v>9.2791578978624514E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9">
-        <f>(C2*C12*C10*C11)^-1</f>
-        <v>1.5278557904067591</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="12"/>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="H4">
+        <f>B6*10^-3/(G20*B14*10^-4)</f>
+        <v>0.57312445839738679</v>
       </c>
       <c r="I4">
-        <f>1/$I$3</f>
-        <v>3.5922800000000006</v>
-      </c>
-      <c r="J4">
-        <f>1/J3</f>
-        <v>10.776840000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="9">
-        <f>C4^-1</f>
-        <v>0.6545120333207437</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B6" s="11"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="12"/>
-      <c r="G6" t="s">
+        <f>(B6*10^-3)/(G21*B14*10^-4)</f>
+        <v>0.51279556803976711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>26.3</v>
+      </c>
+      <c r="D5">
+        <v>46.8</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6">
-        <f>C8*10^-3/(H21*C16*10^-4)</f>
-        <v>0.49124953576918862</v>
-      </c>
-      <c r="J6">
-        <f>(C8*10^-3)/(H22*C16*10^-4)</f>
-        <v>0.43953905831980034</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="H5">
+        <f>1/H4</f>
+        <v>1.7448217142857143</v>
+      </c>
+      <c r="I5">
+        <f>1/I4</f>
+        <v>1.9500948571428574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1.4</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="9">
+        <f>1/(I16*B14*10^-4)</f>
+        <v>6.9593684233968389</v>
+      </c>
+      <c r="I6" s="9">
+        <f>1/(I17*B14*10^-4)</f>
+        <v>3.4796842116984195</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="9">
-        <v>26.3</v>
-      </c>
-      <c r="E7" s="12">
-        <v>46.8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
+        <f>1/H6</f>
+        <v>0.14369120000000002</v>
+      </c>
+      <c r="I7" s="9">
         <f>1/I6</f>
-        <v>2.0356253333333338</v>
-      </c>
-      <c r="J7">
-        <f>1/J6</f>
-        <v>2.2751106666666669</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1.2</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="12"/>
+        <v>0.28738240000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
       <c r="G8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="H8">
+        <f>1/(K16*B14*10^-4)</f>
+        <v>1.3918736846793678</v>
       </c>
       <c r="I8">
-        <f>1/(J17*C16*10^-4)</f>
-        <v>6.9593684233968389</v>
-      </c>
-      <c r="J8">
-        <f>1/(J18*C16*10^-4)</f>
-        <v>3.4796842116984195</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B9" s="11"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="12"/>
-      <c r="G9" t="s">
-        <v>21</v>
+        <f>1/(K17*B14*10^-4)</f>
+        <v>2.3197894744656129E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>0.997</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <f>1/H8</f>
+        <v>0.71845600000000009</v>
       </c>
       <c r="I9">
         <f>1/I8</f>
-        <v>0.14369120000000002</v>
-      </c>
-      <c r="J9">
-        <f>1/J8</f>
-        <v>0.28738240000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B10" s="11" t="s">
+        <v>43.107360000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>4.18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <f>1/(H2+H4+H8)</f>
+        <v>0.29789639024390246</v>
+      </c>
+      <c r="I10">
+        <f>1/(I2+I4+I8)</f>
+        <v>1.8417806161457162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B6*0.001/(B3*(2*(B5*C5+C5*D5)+B5*D5)*0.000001)</f>
+        <v>0.2077835445403923</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>143.69120000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>B14*(1/B3)/(2*0.01*(B5*C5+B5*D5+C5*D5))</f>
+        <v>1.7619822164985144</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="9">
         <v>10</v>
       </c>
-      <c r="C10" s="9">
+      <c r="J16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17">
+        <v>10000</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="9">
+        <v>20</v>
+      </c>
+      <c r="J17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="F18" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E19" s="7"/>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0.98809999999999998</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11">
-        <f>1/(I3+I6+I8)</f>
-        <v>0.12938296610169492</v>
-      </c>
-      <c r="J11">
-        <f>1/(J3+J6+J8)</f>
-        <v>0.24925132075471704</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="9">
-        <v>4.18</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B13" s="11"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="10">
-        <f>C8*0.001/(C4*(2*(C7*D7+D7*E7)+C7*E7)*0.000001)</f>
-        <v>0.17651031983982948</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="9">
-        <v>143.69120000000001</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B17" s="11"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="12"/>
-      <c r="G17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17">
-        <v>250</v>
-      </c>
-      <c r="I17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="14">
-        <f>C16*(1/C4)/(2*0.01*(C7*D7+C7*E7+D7*E7))</f>
-        <v>1.7462533882870432</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="G18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18">
-        <v>750</v>
-      </c>
-      <c r="I18" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="G19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="F21" s="6"/>
-      <c r="G21" t="s">
+      <c r="G20">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
         <v>31</v>
       </c>
-      <c r="H21">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="G22" t="s">
+      <c r="G21">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
         <v>32</v>
       </c>
-      <c r="H22">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="G23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A24" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26">
-        <v>5.2822530159999997E-3</v>
-      </c>
-      <c r="C26" s="3">
-        <v>2.1810521689999999E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27">
-        <v>30</v>
-      </c>
-      <c r="C27">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28">
-        <v>0.6545120333207437</v>
-      </c>
-      <c r="C28">
-        <v>0.36033232677718402</v>
-      </c>
-      <c r="D28" s="22">
-        <f>B28/C28</f>
-        <v>1.8164121969702411</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F18" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>